<commit_message>
Made atomic composition comparison table
</commit_message>
<xml_diff>
--- a/Batch 1_Measured alloy component entry_completed.xlsx
+++ b/Batch 1_Measured alloy component entry_completed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sb3920_ic_ac_uk/Documents/[01] MEng project/[03] Computer calculators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_496D28E7C762BA0E6235547658F9067C88F185DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDEB3401-4E24-483F-8970-3211AECCD7B0}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_496D28E7C762BA0E62355476584E86FFBA4984DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F76AF4-5B9A-4C9C-B3C0-01BF765DEA2D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,15 @@
     <t>Ti(20.0)V(20.0)Nb(20.0)Hf(20.0)Cr(20.0)</t>
   </si>
   <si>
+    <t>Ti</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
+    <t>Nb</t>
+  </si>
+  <si>
     <t>Hf</t>
   </si>
   <si>
@@ -50,12 +56,6 @@
   </si>
   <si>
     <t>Cr</t>
-  </si>
-  <si>
-    <t>Ti</t>
-  </si>
-  <si>
-    <t>Nb</t>
   </si>
 </sst>
 </file>
@@ -175,15 +175,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D95BD366-8F5C-49CA-95F5-F9397A01D730}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:F7" xr:uid="{D95BD366-8F5C-49CA-95F5-F9397A01D730}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A98D1C42-6F64-4B0F-8A77-13A67A173BC2}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:F7" xr:uid="{A98D1C42-6F64-4B0F-8A77-13A67A173BC2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3A9AB020-D5FF-49F5-B446-A8361FD97277}" name="Alloying element"/>
-    <tableColumn id="2" xr3:uid="{7B9911C0-D036-4C8F-8062-2CD90723861B}" name="Ti(38.0)V(15.0)Nb(23.0)Hf(24.0)"/>
-    <tableColumn id="3" xr3:uid="{00F85437-1C2F-4103-95FC-E3DF0E468B08}" name="Ti(25.0)V(25.0)Nb(25.0)Hf(25.0)"/>
-    <tableColumn id="4" xr3:uid="{9D9AF1F0-4003-418E-9DB2-45B3BA14FE59}" name="Ti(20.0)V(20.0)Nb(20.0)Hf(20.0)Si(20.0)"/>
-    <tableColumn id="5" xr3:uid="{9AAA6CBA-41A7-491A-8D76-9BADAAA81918}" name="Ti(38.0)V(15.0)Nb(23.0)Hf(23.0)Si(1.0)"/>
-    <tableColumn id="6" xr3:uid="{C40118B9-9336-46EE-B40B-B61503B0A400}" name="Ti(20.0)V(20.0)Nb(20.0)Hf(20.0)Cr(20.0)"/>
+    <tableColumn id="1" xr3:uid="{842E4063-F95C-4713-835A-38E24A2D936B}" name="Alloying element"/>
+    <tableColumn id="2" xr3:uid="{21B47F57-A44B-4FD9-B62F-F82EA15AA877}" name="Ti(38.0)V(15.0)Nb(23.0)Hf(24.0)"/>
+    <tableColumn id="3" xr3:uid="{3D2B8EA0-03F5-4EE4-858B-4901A224A08C}" name="Ti(25.0)V(25.0)Nb(25.0)Hf(25.0)"/>
+    <tableColumn id="4" xr3:uid="{4F2AB506-9040-4264-BFE8-8FD65E457951}" name="Ti(20.0)V(20.0)Nb(20.0)Hf(20.0)Si(20.0)"/>
+    <tableColumn id="5" xr3:uid="{8CF2C87E-905E-4A8D-B4B6-956680AD3642}" name="Ti(38.0)V(15.0)Nb(23.0)Hf(23.0)Si(1.0)"/>
+    <tableColumn id="6" xr3:uid="{7BBDED19-E690-420F-B8B5-3D7B52BCF5F3}" name="Ti(20.0)V(20.0)Nb(20.0)Hf(20.0)Cr(20.0)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,19 +514,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.83</v>
+        <v>2.09</v>
       </c>
       <c r="C2">
-        <v>1.4</v>
+        <v>1.32</v>
       </c>
       <c r="D2">
-        <v>1.28</v>
+        <v>1.21</v>
       </c>
       <c r="E2">
-        <v>0.87</v>
+        <v>2.09</v>
       </c>
       <c r="F2">
-        <v>1.21</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -534,19 +534,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>4.74</v>
+        <v>0.83</v>
       </c>
       <c r="C3">
-        <v>4.8</v>
+        <v>1.4</v>
       </c>
       <c r="D3">
-        <v>4.5199999999999996</v>
+        <v>1.28</v>
       </c>
       <c r="E3">
-        <v>4.67</v>
+        <v>0.87</v>
       </c>
       <c r="F3">
-        <v>4.13</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -554,19 +554,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.46</v>
       </c>
       <c r="D4">
-        <v>1.1499999999999999</v>
+        <v>2.29</v>
       </c>
       <c r="E4">
-        <v>0.92</v>
+        <v>2.5</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -574,19 +574,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4.74</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>4.67</v>
       </c>
       <c r="F5">
-        <v>1.91</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -594,19 +594,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2.09</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1.32</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1.21</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E6">
-        <v>2.09</v>
+        <v>0.92</v>
       </c>
       <c r="F6">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -614,19 +614,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>2.2799999999999998</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1.46</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2.29</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>2.09</v>
+        <v>1.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>